<commit_message>
can read room coordinates from xlsx file
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Room Coordinates</t>
   </si>
@@ -32,21 +32,50 @@
     <t>(0,0)</t>
   </si>
   <si>
-    <t>(2,3)</t>
-  </si>
-  <si>
-    <t>(4,5)</t>
-  </si>
-  <si>
-    <t>hello</t>
+    <t>Chillers</t>
+  </si>
+  <si>
+    <t>Width:</t>
+  </si>
+  <si>
+    <t>Amount:</t>
+  </si>
+  <si>
+    <t>Length:</t>
+  </si>
+  <si>
+    <t>Boilers</t>
+  </si>
+  <si>
+    <t>AHUs</t>
+  </si>
+  <si>
+    <t>Pumps</t>
+  </si>
+  <si>
+    <t>(4,4)</t>
+  </si>
+  <si>
+    <t>(4,0)</t>
+  </si>
+  <si>
+    <t>(0,4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -62,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -70,12 +99,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,50 +454,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="I2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="L2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="I3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="L3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="F4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="I4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="L4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
can read Chiller number
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -56,10 +56,10 @@
     <t>(4,4)</t>
   </si>
   <si>
-    <t>(4,0)</t>
-  </si>
-  <si>
     <t>(0,4)</t>
+  </si>
+  <si>
+    <t>(2,0)</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,7 +494,9 @@
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5">
+        <v>4</v>
+      </c>
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
@@ -510,7 +512,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -552,7 +554,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
can read chiller number and bounds
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -517,7 +517,9 @@
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5">
+        <v>1.7</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
@@ -538,7 +540,9 @@
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
reads boiler number and boiler bounds from xlsx file
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -59,7 +59,7 @@
     <t>(0,4)</t>
   </si>
   <si>
-    <t>(2,0)</t>
+    <t>(4,0)</t>
   </si>
 </sst>
 </file>
@@ -91,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -161,19 +161,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +467,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,95 +476,101 @@
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="2"/>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="I1" s="2" t="s">
+      <c r="G1" s="2"/>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="L1" s="2" t="s">
+      <c r="J1" s="2"/>
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="7">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4">
+        <v>2</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4"/>
+      <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="L2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="5"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5">
-        <v>1.7</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="I3" s="4" t="s">
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="5"/>
-      <c r="L3" s="4" t="s">
+      <c r="J3" s="4"/>
+      <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="5"/>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="I4" s="6" t="s">
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="L4" s="6" t="s">
+      <c r="J4" s="6"/>
+      <c r="L4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="7"/>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
reads all values from excel, still need to make more efficient
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -467,7 +467,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,11 +516,15 @@
       <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="4"/>
+      <c r="J2" s="4">
+        <v>2</v>
+      </c>
       <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="4"/>
+      <c r="M2" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -541,11 +545,15 @@
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
       <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="4"/>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -566,11 +574,15 @@
       <c r="I4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="6"/>
+      <c r="J4" s="6">
+        <v>2</v>
+      </c>
       <c r="L4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
fully functional, need to optimize
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Room Coordinates</t>
   </si>
@@ -56,10 +56,46 @@
     <t>(4,4)</t>
   </si>
   <si>
-    <t>(0,4)</t>
-  </si>
-  <si>
-    <t>(4,0)</t>
+    <t>(3,5)</t>
+  </si>
+  <si>
+    <t>(3,3)</t>
+  </si>
+  <si>
+    <t>(2,3)</t>
+  </si>
+  <si>
+    <t>(2,2)</t>
+  </si>
+  <si>
+    <t>(3,2)</t>
+  </si>
+  <si>
+    <t>(0,2)</t>
+  </si>
+  <si>
+    <t>(1,2)</t>
+  </si>
+  <si>
+    <t>(1,4)</t>
+  </si>
+  <si>
+    <t>(2,4)</t>
+  </si>
+  <si>
+    <t>(3,4)</t>
+  </si>
+  <si>
+    <t>(4,3)</t>
+  </si>
+  <si>
+    <t>(4,1)</t>
+  </si>
+  <si>
+    <t>(1,1)</t>
+  </si>
+  <si>
+    <t>(1,0)</t>
   </si>
 </sst>
 </file>
@@ -464,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +541,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
@@ -517,24 +553,24 @@
         <v>4</v>
       </c>
       <c r="J2" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>3</v>
@@ -545,19 +581,15 @@
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4">
-        <v>1</v>
-      </c>
+      <c r="J3" s="4"/>
       <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="4">
-        <v>1</v>
-      </c>
+      <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
@@ -569,24 +601,90 @@
         <v>5</v>
       </c>
       <c r="G4" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="6">
-        <v>2</v>
-      </c>
+      <c r="J4" s="6"/>
       <c r="L4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="6">
-        <v>2</v>
-      </c>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
works with for units of only one
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,7 +547,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>4</v>
@@ -581,11 +581,15 @@
       <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="4">
+        <v>2</v>
+      </c>
       <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="4"/>
+      <c r="M3" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -606,11 +610,15 @@
       <c r="I4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="6"/>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
       <c r="L4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="M4" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
finally able to show two units one each
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>4</v>
@@ -588,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="M3" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="M4" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed issue with 1x1 display
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -582,13 +582,13 @@
         <v>3</v>
       </c>
       <c r="J3" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M3" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -617,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="M4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
works for 1 of each 4 different kinds of units
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,13 +553,13 @@
         <v>4</v>
       </c>
       <c r="J2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
works with ALL cases, I believe
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -503,7 +503,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +553,7 @@
         <v>4</v>
       </c>
       <c r="J2" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
intialized variables for 4 new unit types
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>Room Coordinates</t>
   </si>
@@ -32,9 +32,6 @@
     <t>(0,0)</t>
   </si>
   <si>
-    <t>Chillers</t>
-  </si>
-  <si>
     <t>Width:</t>
   </si>
   <si>
@@ -44,15 +41,6 @@
     <t>Length:</t>
   </si>
   <si>
-    <t>Boilers</t>
-  </si>
-  <si>
-    <t>AHUs</t>
-  </si>
-  <si>
-    <t>Pumps</t>
-  </si>
-  <si>
     <t>(4,4)</t>
   </si>
   <si>
@@ -96,6 +84,30 @@
   </si>
   <si>
     <t>(1,0)</t>
+  </si>
+  <si>
+    <t>Unit1</t>
+  </si>
+  <si>
+    <t>Unit 2</t>
+  </si>
+  <si>
+    <t>Unit 3</t>
+  </si>
+  <si>
+    <t>Unit 4</t>
+  </si>
+  <si>
+    <t>Unit 5</t>
+  </si>
+  <si>
+    <t>Unit 6</t>
+  </si>
+  <si>
+    <t>Unit 7</t>
+  </si>
+  <si>
+    <t>Unit 8</t>
   </si>
 </sst>
 </file>
@@ -500,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="X14" sqref="X14:X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,187 +524,275 @@
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2"/>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2"/>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2"/>
       <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="2"/>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="2"/>
+      <c r="U1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="2"/>
+      <c r="X1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" s="2"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="4">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" s="7">
+        <v>2</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="4">
+        <v>1</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" s="4">
+        <v>1</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="4">
+        <v>2</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="4">
+        <v>3</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="4">
+        <v>1</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="4">
+        <v>1</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="6">
+        <v>2</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P4" s="6">
+        <v>1</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S4" s="6">
+        <v>2</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="6">
+        <v>1</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="4">
-        <v>2</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="4">
-        <v>1</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="6">
-        <v>2</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="6">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
8 diff units and dimensions read from excel
</commit_message>
<xml_diff>
--- a/Dimensions.xlsx
+++ b/Dimensions.xlsx
@@ -515,7 +515,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +611,7 @@
         <v>3</v>
       </c>
       <c r="Y2" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>